<commit_message>
Got it compiling under VS2013 again.
</commit_message>
<xml_diff>
--- a/test/scaling.xlsx
+++ b/test/scaling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Scaling</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>GCC 4.8 write over VS2013 read</t>
+  </si>
+  <si>
+    <t>write GCC 4.8 ARMv7 4 core 4 thread ARM Cortex-A15 @ 2.3Ghz</t>
+  </si>
+  <si>
+    <t>read GCC 4.8 ARMv7 4 core 4 thread ARM Cortex-A15 @ 2.3Ghz</t>
   </si>
 </sst>
 </file>
@@ -160,7 +166,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-IE"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -396,11 +402,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="155215744"/>
-        <c:axId val="155246976"/>
+        <c:axId val="132294144"/>
+        <c:axId val="132308992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155215744"/>
+        <c:axId val="132294144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -427,12 +433,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155246976"/>
+        <c:crossAx val="132308992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155246976"/>
+        <c:axId val="132308992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +464,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155215744"/>
+        <c:crossAx val="132294144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -471,7 +477,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -479,7 +485,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-IE"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -620,11 +626,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61684736"/>
-        <c:axId val="61683200"/>
+        <c:axId val="132207360"/>
+        <c:axId val="132209280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61684736"/>
+        <c:axId val="132207360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -656,12 +662,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61683200"/>
+        <c:crossAx val="132209280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61683200"/>
+        <c:axId val="132209280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -693,7 +699,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61684736"/>
+        <c:crossAx val="132207360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -706,7 +712,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1064,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1342,11 +1348,11 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B15" si="5">C14/D14</f>
+        <f t="shared" ref="B14:B17" si="5">C14/D14</f>
         <v>0.22979036330042299</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C15" si="6">H14/E14</f>
+        <f t="shared" ref="C14:C17" si="6">H14/E14</f>
         <v>0.91916145320169196</v>
       </c>
       <c r="D14">
@@ -1381,6 +1387,50 @@
         <v>42351210</v>
       </c>
     </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="5"/>
+        <v>0.23574063965380038</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="6"/>
+        <v>0.94296255861520151</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3801275</v>
+      </c>
+      <c r="H16">
+        <v>3584460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="5"/>
+        <v>1.8573589810194937E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="6"/>
+        <v>7.4294359240779748E-2</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>8885116</v>
+      </c>
+      <c r="H17">
+        <v>660114</v>
+      </c>
+    </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>7</v>
@@ -1689,11 +1739,11 @@
         <v>22</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B34" si="12">C33/D33</f>
+        <f t="shared" ref="B33:B36" si="12">C33/D33</f>
         <v>0.99589349211171696</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:C34" si="13">H33/E33</f>
+        <f t="shared" ref="C33:C36" si="13">H33/E33</f>
         <v>3.9835739684468678</v>
       </c>
       <c r="D33">
@@ -1726,6 +1776,50 @@
       </c>
       <c r="H34">
         <v>98416354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:B36" si="14">C35/D35</f>
+        <v>0.96502362251172635</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C36" si="15">H35/E35</f>
+        <v>3.8600944900469054</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>3356544</v>
+      </c>
+      <c r="H35">
+        <v>12956577</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="14"/>
+        <v>0.90095421566402856</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="15"/>
+        <v>3.6038168626561142</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>4385015</v>
+      </c>
+      <c r="H36">
+        <v>15802791</v>
       </c>
     </row>
     <row r="40" spans="1:8">

</xml_diff>